<commit_message>
code ready for blog
</commit_message>
<xml_diff>
--- a/data/output/data.xlsx
+++ b/data/output/data.xlsx
@@ -472,7 +472,7 @@
         <v>43107</v>
       </c>
       <c r="C2" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D2" t="n">
         <v>6.028571428571429</v>
@@ -492,7 +492,7 @@
         <v>43114</v>
       </c>
       <c r="C3" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D3" t="n">
         <v>4.114285714285715</v>
@@ -512,7 +512,7 @@
         <v>43121</v>
       </c>
       <c r="C4" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D4" t="n">
         <v>4.085714285714286</v>
@@ -532,7 +532,7 @@
         <v>43128</v>
       </c>
       <c r="C5" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D5" t="n">
         <v>7.814285714285715</v>
@@ -572,7 +572,7 @@
         <v>43142</v>
       </c>
       <c r="C7" t="n">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="D7" t="n">
         <v>0.8142857142857142</v>
@@ -592,7 +592,7 @@
         <v>43149</v>
       </c>
       <c r="C8" t="n">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="D8" t="n">
         <v>2.285714285714286</v>
@@ -612,7 +612,7 @@
         <v>43156</v>
       </c>
       <c r="C9" t="n">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="D9" t="n">
         <v>-0.08571428571428573</v>
@@ -632,7 +632,7 @@
         <v>43163</v>
       </c>
       <c r="C10" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D10" t="n">
         <v>-2.657142857142857</v>
@@ -652,7 +652,7 @@
         <v>43170</v>
       </c>
       <c r="C11" t="n">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="D11" t="n">
         <v>7.285714285714286</v>
@@ -672,7 +672,7 @@
         <v>43177</v>
       </c>
       <c r="C12" t="n">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="D12" t="n">
         <v>4.342857142857143</v>
@@ -692,7 +692,7 @@
         <v>43184</v>
       </c>
       <c r="C13" t="n">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="D13" t="n">
         <v>4.528571428571428</v>
@@ -712,7 +712,7 @@
         <v>43191</v>
       </c>
       <c r="C14" t="n">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="D14" t="n">
         <v>6.242857142857143</v>
@@ -732,7 +732,7 @@
         <v>43198</v>
       </c>
       <c r="C15" t="n">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="D15" t="n">
         <v>10.64285714285714</v>
@@ -752,7 +752,7 @@
         <v>43205</v>
       </c>
       <c r="C16" t="n">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="D16" t="n">
         <v>12.2</v>
@@ -772,7 +772,7 @@
         <v>43212</v>
       </c>
       <c r="C17" t="n">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="D17" t="n">
         <v>15.91428571428571</v>
@@ -792,7 +792,7 @@
         <v>43219</v>
       </c>
       <c r="C18" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D18" t="n">
         <v>11.28571428571429</v>
@@ -812,7 +812,7 @@
         <v>43226</v>
       </c>
       <c r="C19" t="n">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="D19" t="n">
         <v>11.78571428571429</v>
@@ -832,7 +832,7 @@
         <v>43233</v>
       </c>
       <c r="C20" t="n">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D20" t="n">
         <v>15.64285714285714</v>
@@ -852,7 +852,7 @@
         <v>43240</v>
       </c>
       <c r="C21" t="n">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="D21" t="n">
         <v>14.55714285714286</v>
@@ -872,7 +872,7 @@
         <v>43247</v>
       </c>
       <c r="C22" t="n">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="D22" t="n">
         <v>19.78571428571428</v>
@@ -892,7 +892,7 @@
         <v>43254</v>
       </c>
       <c r="C23" t="n">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="D23" t="n">
         <v>20.02857142857143</v>
@@ -912,7 +912,7 @@
         <v>43261</v>
       </c>
       <c r="C24" t="n">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D24" t="n">
         <v>19.08571428571429</v>
@@ -932,7 +932,7 @@
         <v>43268</v>
       </c>
       <c r="C25" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D25" t="n">
         <v>16.28571428571428</v>
@@ -952,7 +952,7 @@
         <v>43275</v>
       </c>
       <c r="C26" t="n">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D26" t="n">
         <v>15.85714285714286</v>
@@ -972,7 +972,7 @@
         <v>43282</v>
       </c>
       <c r="C27" t="n">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D27" t="n">
         <v>19.1</v>
@@ -992,7 +992,7 @@
         <v>43289</v>
       </c>
       <c r="C28" t="n">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="D28" t="n">
         <v>19.24285714285714</v>
@@ -1012,7 +1012,7 @@
         <v>43296</v>
       </c>
       <c r="C29" t="n">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D29" t="n">
         <v>18.35714285714286</v>
@@ -1032,7 +1032,7 @@
         <v>43303</v>
       </c>
       <c r="C30" t="n">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="D30" t="n">
         <v>20.3</v>
@@ -1052,7 +1052,7 @@
         <v>43310</v>
       </c>
       <c r="C31" t="n">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="D31" t="n">
         <v>24.35714285714286</v>
@@ -1092,7 +1092,7 @@
         <v>43324</v>
       </c>
       <c r="C33" t="n">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="D33" t="n">
         <v>19.67142857142857</v>
@@ -1112,7 +1112,7 @@
         <v>43331</v>
       </c>
       <c r="C34" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D34" t="n">
         <v>18.6</v>
@@ -1132,7 +1132,7 @@
         <v>43338</v>
       </c>
       <c r="C35" t="n">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="D35" t="n">
         <v>17.15714285714285</v>
@@ -1152,7 +1152,7 @@
         <v>43345</v>
       </c>
       <c r="C36" t="n">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D36" t="n">
         <v>15.04285714285714</v>
@@ -1172,7 +1172,7 @@
         <v>43352</v>
       </c>
       <c r="C37" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D37" t="n">
         <v>17.5</v>
@@ -1192,7 +1192,7 @@
         <v>43359</v>
       </c>
       <c r="C38" t="n">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="D38" t="n">
         <v>15.32857142857143</v>
@@ -1212,7 +1212,7 @@
         <v>43366</v>
       </c>
       <c r="C39" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D39" t="n">
         <v>15.71428571428571</v>
@@ -1232,7 +1232,7 @@
         <v>43373</v>
       </c>
       <c r="C40" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D40" t="n">
         <v>10.45714285714286</v>
@@ -1252,7 +1252,7 @@
         <v>43380</v>
       </c>
       <c r="C41" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D41" t="n">
         <v>12.18571428571429</v>
@@ -1272,7 +1272,7 @@
         <v>43387</v>
       </c>
       <c r="C42" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D42" t="n">
         <v>15.6</v>
@@ -1292,7 +1292,7 @@
         <v>43394</v>
       </c>
       <c r="C43" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D43" t="n">
         <v>12.4</v>
@@ -1312,7 +1312,7 @@
         <v>43401</v>
       </c>
       <c r="C44" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D44" t="n">
         <v>10.04285714285714</v>
@@ -1332,7 +1332,7 @@
         <v>43408</v>
       </c>
       <c r="C45" t="n">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D45" t="n">
         <v>6.714285714285714</v>
@@ -1352,7 +1352,7 @@
         <v>43415</v>
       </c>
       <c r="C46" t="n">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="D46" t="n">
         <v>10.34285714285714</v>
@@ -1372,7 +1372,7 @@
         <v>43422</v>
       </c>
       <c r="C47" t="n">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D47" t="n">
         <v>6.5</v>
@@ -1392,7 +1392,7 @@
         <v>43429</v>
       </c>
       <c r="C48" t="n">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D48" t="n">
         <v>3.414285714285714</v>
@@ -1412,7 +1412,7 @@
         <v>43436</v>
       </c>
       <c r="C49" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D49" t="n">
         <v>7.685714285714285</v>
@@ -1432,7 +1432,7 @@
         <v>43443</v>
       </c>
       <c r="C50" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D50" t="n">
         <v>8.571428571428571</v>
@@ -1452,7 +1452,7 @@
         <v>43450</v>
       </c>
       <c r="C51" t="n">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="D51" t="n">
         <v>1.942857142857143</v>
@@ -1472,7 +1472,7 @@
         <v>43457</v>
       </c>
       <c r="C52" t="n">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="D52" t="n">
         <v>7.614285714285714</v>
@@ -1492,7 +1492,7 @@
         <v>43464</v>
       </c>
       <c r="C53" t="n">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D53" t="n">
         <v>4.971428571428571</v>
@@ -1512,7 +1512,7 @@
         <v>43471</v>
       </c>
       <c r="C54" t="n">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D54" t="n">
         <v>6.314285714285715</v>
@@ -1532,7 +1532,7 @@
         <v>43478</v>
       </c>
       <c r="C55" t="n">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D55" t="n">
         <v>6.428571428571429</v>
@@ -1552,7 +1552,7 @@
         <v>43485</v>
       </c>
       <c r="C56" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D56" t="n">
         <v>2.3</v>
@@ -1572,7 +1572,7 @@
         <v>43492</v>
       </c>
       <c r="C57" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D57" t="n">
         <v>1.028571428571429</v>
@@ -1592,7 +1592,7 @@
         <v>43499</v>
       </c>
       <c r="C58" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D58" t="n">
         <v>1.328571428571429</v>
@@ -1612,7 +1612,7 @@
         <v>43506</v>
       </c>
       <c r="C59" t="n">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="D59" t="n">
         <v>6.014285714285714</v>
@@ -1632,7 +1632,7 @@
         <v>43513</v>
       </c>
       <c r="C60" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D60" t="n">
         <v>5.628571428571428</v>
@@ -1652,7 +1652,7 @@
         <v>43520</v>
       </c>
       <c r="C61" t="n">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="D61" t="n">
         <v>7.514285714285714</v>
@@ -1672,7 +1672,7 @@
         <v>43527</v>
       </c>
       <c r="C62" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D62" t="n">
         <v>8.285714285714286</v>
@@ -1692,7 +1692,7 @@
         <v>43534</v>
       </c>
       <c r="C63" t="n">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="D63" t="n">
         <v>8.27142857142857</v>
@@ -1712,7 +1712,7 @@
         <v>43541</v>
       </c>
       <c r="C64" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D64" t="n">
         <v>7.757142857142857</v>
@@ -1732,7 +1732,7 @@
         <v>43548</v>
       </c>
       <c r="C65" t="n">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="D65" t="n">
         <v>7.157142857142857</v>
@@ -1752,7 +1752,7 @@
         <v>43555</v>
       </c>
       <c r="C66" t="n">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D66" t="n">
         <v>8.742857142857144</v>
@@ -1772,7 +1772,7 @@
         <v>43562</v>
       </c>
       <c r="C67" t="n">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D67" t="n">
         <v>8.800000000000001</v>
@@ -1792,7 +1792,7 @@
         <v>43569</v>
       </c>
       <c r="C68" t="n">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="D68" t="n">
         <v>7.100000000000001</v>
@@ -1812,7 +1812,7 @@
         <v>43576</v>
       </c>
       <c r="C69" t="n">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D69" t="n">
         <v>14.57142857142857</v>
@@ -1832,7 +1832,7 @@
         <v>43583</v>
       </c>
       <c r="C70" t="n">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="D70" t="n">
         <v>13.32857142857143</v>
@@ -1852,7 +1852,7 @@
         <v>43590</v>
       </c>
       <c r="C71" t="n">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="D71" t="n">
         <v>8.657142857142857</v>
@@ -1872,7 +1872,7 @@
         <v>43597</v>
       </c>
       <c r="C72" t="n">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="D72" t="n">
         <v>9.557142857142859</v>
@@ -1892,7 +1892,7 @@
         <v>43604</v>
       </c>
       <c r="C73" t="n">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="D73" t="n">
         <v>12.38571428571429</v>
@@ -1912,7 +1912,7 @@
         <v>43611</v>
       </c>
       <c r="C74" t="n">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D74" t="n">
         <v>13.95714285714286</v>
@@ -1932,7 +1932,7 @@
         <v>43618</v>
       </c>
       <c r="C75" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D75" t="n">
         <v>16.27142857142857</v>
@@ -1952,7 +1952,7 @@
         <v>43625</v>
       </c>
       <c r="C76" t="n">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D76" t="n">
         <v>16.02857142857143</v>
@@ -1972,7 +1972,7 @@
         <v>43632</v>
       </c>
       <c r="C77" t="n">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="D77" t="n">
         <v>15.91428571428571</v>
@@ -1992,7 +1992,7 @@
         <v>43639</v>
       </c>
       <c r="C78" t="n">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="D78" t="n">
         <v>18.61428571428572</v>
@@ -2012,7 +2012,7 @@
         <v>43646</v>
       </c>
       <c r="C79" t="n">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D79" t="n">
         <v>21.21428571428572</v>
@@ -2032,7 +2032,7 @@
         <v>43653</v>
       </c>
       <c r="C80" t="n">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="D80" t="n">
         <v>16.55714285714286</v>
@@ -2052,7 +2052,7 @@
         <v>43660</v>
       </c>
       <c r="C81" t="n">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D81" t="n">
         <v>15.9</v>
@@ -2072,7 +2072,7 @@
         <v>43667</v>
       </c>
       <c r="C82" t="n">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D82" t="n">
         <v>17.85714285714286</v>
@@ -2092,7 +2092,7 @@
         <v>43674</v>
       </c>
       <c r="C83" t="n">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="D83" t="n">
         <v>24.42857142857143</v>
@@ -2112,7 +2112,7 @@
         <v>43681</v>
       </c>
       <c r="C84" t="n">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="D84" t="n">
         <v>18.94285714285714</v>
@@ -2132,7 +2132,7 @@
         <v>43688</v>
       </c>
       <c r="C85" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D85" t="n">
         <v>19.38571428571428</v>
@@ -2152,7 +2152,7 @@
         <v>43695</v>
       </c>
       <c r="C86" t="n">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="D86" t="n">
         <v>16.54285714285714</v>
@@ -2172,7 +2172,7 @@
         <v>43702</v>
       </c>
       <c r="C87" t="n">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="D87" t="n">
         <v>17.45714285714286</v>
@@ -2192,7 +2192,7 @@
         <v>43709</v>
       </c>
       <c r="C88" t="n">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D88" t="n">
         <v>20.1</v>
@@ -2212,7 +2212,7 @@
         <v>43716</v>
       </c>
       <c r="C89" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D89" t="n">
         <v>14.45714285714286</v>
@@ -2232,7 +2232,7 @@
         <v>43723</v>
       </c>
       <c r="C90" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D90" t="n">
         <v>14.57142857142857</v>
@@ -2252,7 +2252,7 @@
         <v>43730</v>
       </c>
       <c r="C91" t="n">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D91" t="n">
         <v>13.4</v>
@@ -2272,7 +2272,7 @@
         <v>43737</v>
       </c>
       <c r="C92" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="D92" t="n">
         <v>15.45714285714286</v>
@@ -2292,7 +2292,7 @@
         <v>43744</v>
       </c>
       <c r="C93" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D93" t="n">
         <v>11.54285714285714</v>
@@ -2312,7 +2312,7 @@
         <v>43751</v>
       </c>
       <c r="C94" t="n">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="D94" t="n">
         <v>12.95714285714286</v>
@@ -2332,7 +2332,7 @@
         <v>43758</v>
       </c>
       <c r="C95" t="n">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D95" t="n">
         <v>13.08571428571429</v>
@@ -2352,7 +2352,7 @@
         <v>43765</v>
       </c>
       <c r="C96" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D96" t="n">
         <v>12.75714285714286</v>
@@ -2372,7 +2372,7 @@
         <v>43772</v>
       </c>
       <c r="C97" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D97" t="n">
         <v>7.357142857142857</v>
@@ -2392,7 +2392,7 @@
         <v>43779</v>
       </c>
       <c r="C98" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D98" t="n">
         <v>7.114285714285714</v>
@@ -2412,7 +2412,7 @@
         <v>43786</v>
       </c>
       <c r="C99" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D99" t="n">
         <v>5</v>
@@ -2432,7 +2432,7 @@
         <v>43793</v>
       </c>
       <c r="C100" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D100" t="n">
         <v>4.742857142857143</v>
@@ -2452,7 +2452,7 @@
         <v>43800</v>
       </c>
       <c r="C101" t="n">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="D101" t="n">
         <v>5.985714285714286</v>
@@ -2472,7 +2472,7 @@
         <v>43807</v>
       </c>
       <c r="C102" t="n">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="D102" t="n">
         <v>5.371428571428572</v>
@@ -2492,7 +2492,7 @@
         <v>43814</v>
       </c>
       <c r="C103" t="n">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="D103" t="n">
         <v>5.814285714285715</v>
@@ -2512,7 +2512,7 @@
         <v>43821</v>
       </c>
       <c r="C104" t="n">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="D104" t="n">
         <v>8.514285714285714</v>
@@ -2532,7 +2532,7 @@
         <v>43828</v>
       </c>
       <c r="C105" t="n">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D105" t="n">
         <v>4.885714285714286</v>
@@ -2552,7 +2552,7 @@
         <v>43835</v>
       </c>
       <c r="C106" t="n">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D106" t="n">
         <v>4.957142857142857</v>
@@ -2592,7 +2592,7 @@
         <v>43849</v>
       </c>
       <c r="C108" t="n">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="D108" t="n">
         <v>7.328571428571428</v>
@@ -2612,7 +2612,7 @@
         <v>43856</v>
       </c>
       <c r="C109" t="n">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="D109" t="n">
         <v>3.071428571428572</v>
@@ -2632,7 +2632,7 @@
         <v>43863</v>
       </c>
       <c r="C110" t="n">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="D110" t="n">
         <v>8.357142857142858</v>
@@ -2652,7 +2652,7 @@
         <v>43870</v>
       </c>
       <c r="C111" t="n">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D111" t="n">
         <v>6.428571428571429</v>
@@ -2672,7 +2672,7 @@
         <v>43877</v>
       </c>
       <c r="C112" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D112" t="n">
         <v>7.928571428571429</v>
@@ -2692,7 +2692,7 @@
         <v>43884</v>
       </c>
       <c r="C113" t="n">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D113" t="n">
         <v>7.899999999999999</v>
@@ -2712,7 +2712,7 @@
         <v>43891</v>
       </c>
       <c r="C114" t="n">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D114" t="n">
         <v>5.742857142857142</v>
@@ -2732,7 +2732,7 @@
         <v>43898</v>
       </c>
       <c r="C115" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D115" t="n">
         <v>6.2</v>
@@ -2752,7 +2752,7 @@
         <v>43905</v>
       </c>
       <c r="C116" t="n">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="D116" t="n">
         <v>8.6</v>
@@ -2772,7 +2772,7 @@
         <v>43912</v>
       </c>
       <c r="C117" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D117" t="n">
         <v>7.285714285714286</v>
@@ -2792,7 +2792,7 @@
         <v>43919</v>
       </c>
       <c r="C118" t="n">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="D118" t="n">
         <v>6.042857142857143</v>
@@ -2812,7 +2812,7 @@
         <v>43926</v>
       </c>
       <c r="C119" t="n">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="D119" t="n">
         <v>6.471428571428571</v>
@@ -2832,7 +2832,7 @@
         <v>43933</v>
       </c>
       <c r="C120" t="n">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="D120" t="n">
         <v>13.21428571428571</v>
@@ -2852,7 +2852,7 @@
         <v>43940</v>
       </c>
       <c r="C121" t="n">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="D121" t="n">
         <v>9.971428571428572</v>
@@ -2872,7 +2872,7 @@
         <v>43947</v>
       </c>
       <c r="C122" t="n">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="D122" t="n">
         <v>12.68571428571429</v>
@@ -2892,7 +2892,7 @@
         <v>43954</v>
       </c>
       <c r="C123" t="n">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="D123" t="n">
         <v>10.97142857142857</v>
@@ -2912,7 +2912,7 @@
         <v>43961</v>
       </c>
       <c r="C124" t="n">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="D124" t="n">
         <v>12.44285714285714</v>
@@ -2952,7 +2952,7 @@
         <v>43975</v>
       </c>
       <c r="C126" t="n">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="D126" t="n">
         <v>16.38571428571429</v>
@@ -2972,7 +2972,7 @@
         <v>43982</v>
       </c>
       <c r="C127" t="n">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="D127" t="n">
         <v>16</v>

</xml_diff>

<commit_message>
code adjusted to new dataset
</commit_message>
<xml_diff>
--- a/data/output/data.xlsx
+++ b/data/output/data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F127"/>
+  <dimension ref="A1:H127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,12 +455,22 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>duration_sunshine</t>
+          <t>sunshine_duration</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>duration_rainfall</t>
+          <t>rainfall_duration</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>avg_air_pressure</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>avg_cloudiness</t>
         </is>
       </c>
     </row>
@@ -478,10 +488,16 @@
         <v>6.028571428571429</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9257142857142858</v>
+        <v>1.542857142857143</v>
       </c>
       <c r="F2" t="n">
-        <v>1.902857142857143</v>
+        <v>3.171428571428571</v>
+      </c>
+      <c r="G2" t="n">
+        <v>10028.28571428571</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1112668.857142857</v>
       </c>
     </row>
     <row r="3">
@@ -492,16 +508,22 @@
         <v>43114</v>
       </c>
       <c r="C3" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D3" t="n">
         <v>4.114285714285715</v>
       </c>
       <c r="E3" t="n">
-        <v>1.011428571428571</v>
+        <v>1.685714285714286</v>
       </c>
       <c r="F3" t="n">
-        <v>0.4971428571428572</v>
+        <v>0.8285714285714285</v>
+      </c>
+      <c r="G3" t="n">
+        <v>10187.14285714286</v>
+      </c>
+      <c r="H3" t="n">
+        <v>698410.5714285715</v>
       </c>
     </row>
     <row r="4">
@@ -512,16 +534,22 @@
         <v>43121</v>
       </c>
       <c r="C4" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D4" t="n">
         <v>4.085714285714286</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9857142857142858</v>
+        <v>1.642857142857143</v>
       </c>
       <c r="F4" t="n">
-        <v>2.562857142857143</v>
+        <v>4.271428571428571</v>
+      </c>
+      <c r="G4" t="n">
+        <v>10015.57142857143</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1253953.714285714</v>
       </c>
     </row>
     <row r="5">
@@ -538,10 +566,16 @@
         <v>7.814285714285715</v>
       </c>
       <c r="E5" t="n">
-        <v>0.5914285714285715</v>
+        <v>0.9857142857142858</v>
       </c>
       <c r="F5" t="n">
-        <v>1.174285714285714</v>
+        <v>1.957142857142857</v>
+      </c>
+      <c r="G5" t="n">
+        <v>10176.85714285714</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1269826.857142857</v>
       </c>
     </row>
     <row r="6">
@@ -552,16 +586,22 @@
         <v>43135</v>
       </c>
       <c r="C6" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D6" t="n">
         <v>4.5</v>
       </c>
       <c r="E6" t="n">
-        <v>1.26</v>
+        <v>2.1</v>
       </c>
       <c r="F6" t="n">
-        <v>1.731428571428571</v>
+        <v>2.885714285714286</v>
+      </c>
+      <c r="G6" t="n">
+        <v>10122.85714285714</v>
+      </c>
+      <c r="H6" t="n">
+        <v>953969.5714285715</v>
       </c>
     </row>
     <row r="7">
@@ -578,10 +618,16 @@
         <v>0.8142857142857142</v>
       </c>
       <c r="E7" t="n">
-        <v>2.725714285714286</v>
+        <v>4.542857142857143</v>
       </c>
       <c r="F7" t="n">
-        <v>0.3257142857142857</v>
+        <v>0.5428571428571428</v>
+      </c>
+      <c r="G7" t="n">
+        <v>10151</v>
+      </c>
+      <c r="H7" t="n">
+        <v>732553.8571428572</v>
       </c>
     </row>
     <row r="8">
@@ -592,16 +638,22 @@
         <v>43149</v>
       </c>
       <c r="C8" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D8" t="n">
         <v>2.285714285714286</v>
       </c>
       <c r="E8" t="n">
-        <v>4.2</v>
+        <v>7</v>
       </c>
       <c r="F8" t="n">
-        <v>0.3257142857142857</v>
+        <v>0.5428571428571428</v>
+      </c>
+      <c r="G8" t="n">
+        <v>10172.42857142857</v>
+      </c>
+      <c r="H8" t="n">
+        <v>720779</v>
       </c>
     </row>
     <row r="9">
@@ -612,16 +664,22 @@
         <v>43156</v>
       </c>
       <c r="C9" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D9" t="n">
         <v>-0.08571428571428573</v>
       </c>
       <c r="E9" t="n">
-        <v>4.011428571428572</v>
+        <v>6.685714285714285</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>10246</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1072903</v>
       </c>
     </row>
     <row r="10">
@@ -632,16 +690,22 @@
         <v>43163</v>
       </c>
       <c r="C10" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D10" t="n">
         <v>-2.657142857142857</v>
       </c>
       <c r="E10" t="n">
-        <v>3.608571428571428</v>
+        <v>6.014285714285714</v>
       </c>
       <c r="F10" t="n">
-        <v>0.1885714285714286</v>
+        <v>0.3142857142857143</v>
+      </c>
+      <c r="G10" t="n">
+        <v>10106.42857142857</v>
+      </c>
+      <c r="H10" t="n">
+        <v>636983.8571428572</v>
       </c>
     </row>
     <row r="11">
@@ -658,10 +722,16 @@
         <v>7.285714285714286</v>
       </c>
       <c r="E11" t="n">
-        <v>2.357142857142857</v>
+        <v>3.928571428571428</v>
       </c>
       <c r="F11" t="n">
-        <v>1.705714285714286</v>
+        <v>2.842857142857143</v>
+      </c>
+      <c r="G11" t="n">
+        <v>9962.285714285714</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1125255.142857143</v>
       </c>
     </row>
     <row r="12">
@@ -678,10 +748,16 @@
         <v>4.342857142857143</v>
       </c>
       <c r="E12" t="n">
-        <v>1.834285714285714</v>
+        <v>3.057142857142857</v>
       </c>
       <c r="F12" t="n">
-        <v>1.122857142857143</v>
+        <v>1.871428571428571</v>
+      </c>
+      <c r="G12" t="n">
+        <v>10035</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1265555.428571429</v>
       </c>
     </row>
     <row r="13">
@@ -692,16 +768,22 @@
         <v>43184</v>
       </c>
       <c r="C13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D13" t="n">
         <v>4.528571428571428</v>
       </c>
       <c r="E13" t="n">
-        <v>3.874285714285714</v>
+        <v>6.457142857142857</v>
       </c>
       <c r="F13" t="n">
-        <v>0.3771428571428572</v>
+        <v>0.6285714285714287</v>
+      </c>
+      <c r="G13" t="n">
+        <v>10143</v>
+      </c>
+      <c r="H13" t="n">
+        <v>511123.5714285714</v>
       </c>
     </row>
     <row r="14">
@@ -712,16 +794,22 @@
         <v>43191</v>
       </c>
       <c r="C14" t="n">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D14" t="n">
         <v>6.242857142857143</v>
       </c>
       <c r="E14" t="n">
-        <v>1.68</v>
+        <v>2.8</v>
       </c>
       <c r="F14" t="n">
-        <v>2.374285714285715</v>
+        <v>3.957142857142857</v>
+      </c>
+      <c r="G14" t="n">
+        <v>10058.28571428571</v>
+      </c>
+      <c r="H14" t="n">
+        <v>983982.5714285715</v>
       </c>
     </row>
     <row r="15">
@@ -732,16 +820,22 @@
         <v>43198</v>
       </c>
       <c r="C15" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D15" t="n">
         <v>10.64285714285714</v>
       </c>
       <c r="E15" t="n">
-        <v>3.728571428571429</v>
+        <v>6.214285714285714</v>
       </c>
       <c r="F15" t="n">
-        <v>0.8657142857142857</v>
+        <v>1.442857142857143</v>
+      </c>
+      <c r="G15" t="n">
+        <v>10069.57142857143</v>
+      </c>
+      <c r="H15" t="n">
+        <v>1269669.571428571</v>
       </c>
     </row>
     <row r="16">
@@ -752,16 +846,22 @@
         <v>43205</v>
       </c>
       <c r="C16" t="n">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D16" t="n">
         <v>12.2</v>
       </c>
       <c r="E16" t="n">
-        <v>1.508571428571428</v>
+        <v>2.514285714285715</v>
       </c>
       <c r="F16" t="n">
-        <v>0.6942857142857142</v>
+        <v>1.157142857142857</v>
+      </c>
+      <c r="G16" t="n">
+        <v>10078</v>
+      </c>
+      <c r="H16" t="n">
+        <v>1266555.428571429</v>
       </c>
     </row>
     <row r="17">
@@ -772,16 +872,22 @@
         <v>43212</v>
       </c>
       <c r="C17" t="n">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="D17" t="n">
         <v>15.91428571428571</v>
       </c>
       <c r="E17" t="n">
-        <v>7.131428571428572</v>
+        <v>11.88571428571429</v>
       </c>
       <c r="F17" t="n">
-        <v>0.01714285714285714</v>
+        <v>0.02857142857142857</v>
+      </c>
+      <c r="G17" t="n">
+        <v>10214.85714285714</v>
+      </c>
+      <c r="H17" t="n">
+        <v>667633.5714285715</v>
       </c>
     </row>
     <row r="18">
@@ -792,16 +898,22 @@
         <v>43219</v>
       </c>
       <c r="C18" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D18" t="n">
         <v>11.28571428571429</v>
       </c>
       <c r="E18" t="n">
-        <v>2.537142857142857</v>
+        <v>4.228571428571429</v>
       </c>
       <c r="F18" t="n">
-        <v>0.9171428571428571</v>
+        <v>1.528571428571428</v>
+      </c>
+      <c r="G18" t="n">
+        <v>10115.71428571429</v>
+      </c>
+      <c r="H18" t="n">
+        <v>982268.1428571428</v>
       </c>
     </row>
     <row r="19">
@@ -812,16 +924,22 @@
         <v>43226</v>
       </c>
       <c r="C19" t="n">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D19" t="n">
         <v>11.78571428571429</v>
       </c>
       <c r="E19" t="n">
-        <v>6.497142857142856</v>
+        <v>10.82857142857143</v>
       </c>
       <c r="F19" t="n">
-        <v>1.954285714285714</v>
+        <v>3.257142857142857</v>
+      </c>
+      <c r="G19" t="n">
+        <v>10154.14285714286</v>
+      </c>
+      <c r="H19" t="n">
+        <v>1247142.857142857</v>
       </c>
     </row>
     <row r="20">
@@ -832,16 +950,22 @@
         <v>43233</v>
       </c>
       <c r="C20" t="n">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D20" t="n">
         <v>15.64285714285714</v>
       </c>
       <c r="E20" t="n">
-        <v>5.742857142857143</v>
+        <v>9.571428571428571</v>
       </c>
       <c r="F20" t="n">
-        <v>0.5742857142857142</v>
+        <v>0.9571428571428571</v>
+      </c>
+      <c r="G20" t="n">
+        <v>10133.14285714286</v>
+      </c>
+      <c r="H20" t="n">
+        <v>3641.142857142857</v>
       </c>
     </row>
     <row r="21">
@@ -852,16 +976,22 @@
         <v>43240</v>
       </c>
       <c r="C21" t="n">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D21" t="n">
         <v>14.55714285714286</v>
       </c>
       <c r="E21" t="n">
-        <v>5.014285714285714</v>
+        <v>8.357142857142858</v>
       </c>
       <c r="F21" t="n">
-        <v>0.02571428571428571</v>
+        <v>0.04285714285714286</v>
+      </c>
+      <c r="G21" t="n">
+        <v>10201</v>
+      </c>
+      <c r="H21" t="n">
+        <v>582410.1428571428</v>
       </c>
     </row>
     <row r="22">
@@ -872,16 +1002,22 @@
         <v>43247</v>
       </c>
       <c r="C22" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D22" t="n">
         <v>19.78571428571428</v>
       </c>
       <c r="E22" t="n">
-        <v>3.985714285714285</v>
+        <v>6.642857142857143</v>
       </c>
       <c r="F22" t="n">
-        <v>0.3514285714285714</v>
+        <v>0.5857142857142856</v>
+      </c>
+      <c r="G22" t="n">
+        <v>10175.71428571429</v>
+      </c>
+      <c r="H22" t="n">
+        <v>839680.8571428572</v>
       </c>
     </row>
     <row r="23">
@@ -892,16 +1028,22 @@
         <v>43254</v>
       </c>
       <c r="C23" t="n">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D23" t="n">
         <v>20.02857142857143</v>
       </c>
       <c r="E23" t="n">
-        <v>3.582857142857143</v>
+        <v>5.971428571428571</v>
       </c>
       <c r="F23" t="n">
-        <v>0.6257142857142857</v>
+        <v>1.042857142857143</v>
+      </c>
+      <c r="G23" t="n">
+        <v>10158.71428571429</v>
+      </c>
+      <c r="H23" t="n">
+        <v>966555.1428571428</v>
       </c>
     </row>
     <row r="24">
@@ -912,16 +1054,22 @@
         <v>43261</v>
       </c>
       <c r="C24" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D24" t="n">
         <v>19.08571428571429</v>
       </c>
       <c r="E24" t="n">
-        <v>5.168571428571428</v>
+        <v>8.614285714285714</v>
       </c>
       <c r="F24" t="n">
-        <v>0.3085714285714286</v>
+        <v>0.5142857142857143</v>
+      </c>
+      <c r="G24" t="n">
+        <v>10143</v>
+      </c>
+      <c r="H24" t="n">
+        <v>916552.1428571428</v>
       </c>
     </row>
     <row r="25">
@@ -938,10 +1086,16 @@
         <v>16.28571428571428</v>
       </c>
       <c r="E25" t="n">
-        <v>2.914285714285714</v>
+        <v>4.857142857142857</v>
       </c>
       <c r="F25" t="n">
-        <v>0.1028571428571429</v>
+        <v>0.1714285714285714</v>
+      </c>
+      <c r="G25" t="n">
+        <v>10152.42857142857</v>
+      </c>
+      <c r="H25" t="n">
+        <v>984111</v>
       </c>
     </row>
     <row r="26">
@@ -952,16 +1106,22 @@
         <v>43275</v>
       </c>
       <c r="C26" t="n">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="D26" t="n">
         <v>15.85714285714286</v>
       </c>
       <c r="E26" t="n">
-        <v>2.142857142857143</v>
+        <v>3.571428571428572</v>
       </c>
       <c r="F26" t="n">
         <v>0</v>
+      </c>
+      <c r="G26" t="n">
+        <v>10227.57142857143</v>
+      </c>
+      <c r="H26" t="n">
+        <v>962398.2857142857</v>
       </c>
     </row>
     <row r="27">
@@ -972,16 +1132,22 @@
         <v>43282</v>
       </c>
       <c r="C27" t="n">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D27" t="n">
         <v>19.1</v>
       </c>
       <c r="E27" t="n">
-        <v>8.142857142857142</v>
+        <v>13.57142857142857</v>
       </c>
       <c r="F27" t="n">
         <v>0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>10217.14285714286</v>
+      </c>
+      <c r="H27" t="n">
+        <v>661571.4285714285</v>
       </c>
     </row>
     <row r="28">
@@ -992,16 +1158,22 @@
         <v>43289</v>
       </c>
       <c r="C28" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D28" t="n">
         <v>19.24285714285714</v>
       </c>
       <c r="E28" t="n">
-        <v>7.628571428571428</v>
+        <v>12.71428571428571</v>
       </c>
       <c r="F28" t="n">
         <v>0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>10191.85714285714</v>
+      </c>
+      <c r="H28" t="n">
+        <v>36394.42857142857</v>
       </c>
     </row>
     <row r="29">
@@ -1012,16 +1184,22 @@
         <v>43296</v>
       </c>
       <c r="C29" t="n">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D29" t="n">
         <v>18.35714285714286</v>
       </c>
       <c r="E29" t="n">
-        <v>5.622857142857143</v>
+        <v>9.37142857142857</v>
       </c>
       <c r="F29" t="n">
-        <v>0.03428571428571429</v>
+        <v>0.05714285714285715</v>
+      </c>
+      <c r="G29" t="n">
+        <v>10198</v>
+      </c>
+      <c r="H29" t="n">
+        <v>933314.4285714285</v>
       </c>
     </row>
     <row r="30">
@@ -1032,16 +1210,22 @@
         <v>43303</v>
       </c>
       <c r="C30" t="n">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D30" t="n">
         <v>20.3</v>
       </c>
       <c r="E30" t="n">
-        <v>7.140000000000001</v>
+        <v>11.9</v>
       </c>
       <c r="F30" t="n">
         <v>0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>10151.85714285714</v>
+      </c>
+      <c r="H30" t="n">
+        <v>622231.8571428572</v>
       </c>
     </row>
     <row r="31">
@@ -1052,16 +1236,22 @@
         <v>43310</v>
       </c>
       <c r="C31" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D31" t="n">
         <v>24.35714285714286</v>
       </c>
       <c r="E31" t="n">
-        <v>5.905714285714285</v>
+        <v>9.842857142857143</v>
       </c>
       <c r="F31" t="n">
-        <v>0.1457142857142857</v>
+        <v>0.2428571428571429</v>
+      </c>
+      <c r="G31" t="n">
+        <v>10132.57142857143</v>
+      </c>
+      <c r="H31" t="n">
+        <v>206236.8571428571</v>
       </c>
     </row>
     <row r="32">
@@ -1072,16 +1262,22 @@
         <v>43317</v>
       </c>
       <c r="C32" t="n">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D32" t="n">
         <v>22.05714285714286</v>
       </c>
       <c r="E32" t="n">
-        <v>6.694285714285714</v>
+        <v>11.15714285714286</v>
       </c>
       <c r="F32" t="n">
         <v>0</v>
+      </c>
+      <c r="G32" t="n">
+        <v>10201</v>
+      </c>
+      <c r="H32" t="n">
+        <v>1221866.285714286</v>
       </c>
     </row>
     <row r="33">
@@ -1092,16 +1288,22 @@
         <v>43324</v>
       </c>
       <c r="C33" t="n">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D33" t="n">
         <v>19.67142857142857</v>
       </c>
       <c r="E33" t="n">
-        <v>4.62</v>
+        <v>7.7</v>
       </c>
       <c r="F33" t="n">
-        <v>0.9942857142857143</v>
+        <v>1.657142857142857</v>
+      </c>
+      <c r="G33" t="n">
+        <v>10142.28571428571</v>
+      </c>
+      <c r="H33" t="n">
+        <v>479651.1428571428</v>
       </c>
     </row>
     <row r="34">
@@ -1118,10 +1320,16 @@
         <v>18.6</v>
       </c>
       <c r="E34" t="n">
-        <v>2.751428571428572</v>
+        <v>4.585714285714286</v>
       </c>
       <c r="F34" t="n">
-        <v>0.5228571428571429</v>
+        <v>0.8714285714285713</v>
+      </c>
+      <c r="G34" t="n">
+        <v>10161.42857142857</v>
+      </c>
+      <c r="H34" t="n">
+        <v>1253666.857142857</v>
       </c>
     </row>
     <row r="35">
@@ -1132,16 +1340,22 @@
         <v>43338</v>
       </c>
       <c r="C35" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D35" t="n">
         <v>17.15714285714285</v>
       </c>
       <c r="E35" t="n">
-        <v>3.557142857142857</v>
+        <v>5.928571428571429</v>
       </c>
       <c r="F35" t="n">
-        <v>0.9857142857142858</v>
+        <v>1.642857142857143</v>
+      </c>
+      <c r="G35" t="n">
+        <v>10148.42857142857</v>
+      </c>
+      <c r="H35" t="n">
+        <v>1221109.571428571</v>
       </c>
     </row>
     <row r="36">
@@ -1152,16 +1366,22 @@
         <v>43345</v>
       </c>
       <c r="C36" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D36" t="n">
         <v>15.04285714285714</v>
       </c>
       <c r="E36" t="n">
-        <v>3.36</v>
+        <v>5.600000000000001</v>
       </c>
       <c r="F36" t="n">
-        <v>0.3942857142857143</v>
+        <v>0.6571428571428571</v>
+      </c>
+      <c r="G36" t="n">
+        <v>10200.42857142857</v>
+      </c>
+      <c r="H36" t="n">
+        <v>1253660.285714286</v>
       </c>
     </row>
     <row r="37">
@@ -1172,16 +1392,22 @@
         <v>43352</v>
       </c>
       <c r="C37" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D37" t="n">
         <v>17.5</v>
       </c>
       <c r="E37" t="n">
-        <v>2.357142857142857</v>
+        <v>3.928571428571428</v>
       </c>
       <c r="F37" t="n">
-        <v>0.7628571428571428</v>
+        <v>1.271428571428572</v>
+      </c>
+      <c r="G37" t="n">
+        <v>10166.14285714286</v>
+      </c>
+      <c r="H37" t="n">
+        <v>1254098.285714286</v>
       </c>
     </row>
     <row r="38">
@@ -1198,10 +1424,16 @@
         <v>15.32857142857143</v>
       </c>
       <c r="E38" t="n">
-        <v>2.914285714285714</v>
+        <v>4.857142857142857</v>
       </c>
       <c r="F38" t="n">
-        <v>0.1114285714285714</v>
+        <v>0.1857142857142857</v>
+      </c>
+      <c r="G38" t="n">
+        <v>10211.57142857143</v>
+      </c>
+      <c r="H38" t="n">
+        <v>1268926.571428571</v>
       </c>
     </row>
     <row r="39">
@@ -1218,10 +1450,16 @@
         <v>15.71428571428571</v>
       </c>
       <c r="E39" t="n">
-        <v>3.814285714285714</v>
+        <v>6.357142857142857</v>
       </c>
       <c r="F39" t="n">
-        <v>1.534285714285714</v>
+        <v>2.557142857142857</v>
+      </c>
+      <c r="G39" t="n">
+        <v>10140.57142857143</v>
+      </c>
+      <c r="H39" t="n">
+        <v>1181098</v>
       </c>
     </row>
     <row r="40">
@@ -1238,10 +1476,16 @@
         <v>10.45714285714286</v>
       </c>
       <c r="E40" t="n">
-        <v>5.597142857142857</v>
+        <v>9.328571428571427</v>
       </c>
       <c r="F40" t="n">
-        <v>0.02571428571428571</v>
+        <v>0.04285714285714286</v>
+      </c>
+      <c r="G40" t="n">
+        <v>10289.42857142857</v>
+      </c>
+      <c r="H40" t="n">
+        <v>505939.2857142857</v>
       </c>
     </row>
     <row r="41">
@@ -1252,16 +1496,22 @@
         <v>43380</v>
       </c>
       <c r="C41" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D41" t="n">
         <v>12.18571428571429</v>
       </c>
       <c r="E41" t="n">
-        <v>3.985714285714286</v>
+        <v>6.642857142857143</v>
       </c>
       <c r="F41" t="n">
-        <v>0.6257142857142858</v>
+        <v>1.042857142857143</v>
+      </c>
+      <c r="G41" t="n">
+        <v>10189.85714285714</v>
+      </c>
+      <c r="H41" t="n">
+        <v>1109510.857142857</v>
       </c>
     </row>
     <row r="42">
@@ -1272,16 +1522,22 @@
         <v>43387</v>
       </c>
       <c r="C42" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D42" t="n">
         <v>15.6</v>
       </c>
       <c r="E42" t="n">
-        <v>5.057142857142857</v>
+        <v>8.428571428571429</v>
       </c>
       <c r="F42" t="n">
-        <v>0.04285714285714286</v>
+        <v>0.07142857142857142</v>
+      </c>
+      <c r="G42" t="n">
+        <v>10157.14285714286</v>
+      </c>
+      <c r="H42" t="n">
+        <v>1244969.428571429</v>
       </c>
     </row>
     <row r="43">
@@ -1292,16 +1548,22 @@
         <v>43394</v>
       </c>
       <c r="C43" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D43" t="n">
         <v>12.4</v>
       </c>
       <c r="E43" t="n">
-        <v>3.625714285714285</v>
+        <v>6.042857142857143</v>
       </c>
       <c r="F43" t="n">
         <v>0</v>
+      </c>
+      <c r="G43" t="n">
+        <v>10227.28571428571</v>
+      </c>
+      <c r="H43" t="n">
+        <v>955368.2857142857</v>
       </c>
     </row>
     <row r="44">
@@ -1312,16 +1574,22 @@
         <v>43401</v>
       </c>
       <c r="C44" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D44" t="n">
         <v>10.04285714285714</v>
       </c>
       <c r="E44" t="n">
-        <v>2.185714285714285</v>
+        <v>3.642857142857143</v>
       </c>
       <c r="F44" t="n">
-        <v>0.6171428571428572</v>
+        <v>1.028571428571429</v>
+      </c>
+      <c r="G44" t="n">
+        <v>10187.42857142857</v>
+      </c>
+      <c r="H44" t="n">
+        <v>841264.7142857143</v>
       </c>
     </row>
     <row r="45">
@@ -1332,16 +1600,22 @@
         <v>43408</v>
       </c>
       <c r="C45" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D45" t="n">
         <v>6.714285714285714</v>
       </c>
       <c r="E45" t="n">
-        <v>2.391428571428572</v>
+        <v>3.985714285714285</v>
       </c>
       <c r="F45" t="n">
-        <v>1.902857142857143</v>
+        <v>3.171428571428572</v>
+      </c>
+      <c r="G45" t="n">
+        <v>10112.71428571429</v>
+      </c>
+      <c r="H45" t="n">
+        <v>1268352.142857143</v>
       </c>
     </row>
     <row r="46">
@@ -1352,16 +1626,22 @@
         <v>43415</v>
       </c>
       <c r="C46" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D46" t="n">
         <v>10.34285714285714</v>
       </c>
       <c r="E46" t="n">
-        <v>1.842857142857143</v>
+        <v>3.071428571428572</v>
       </c>
       <c r="F46" t="n">
-        <v>0.9257142857142856</v>
+        <v>1.542857142857143</v>
+      </c>
+      <c r="G46" t="n">
+        <v>10079</v>
+      </c>
+      <c r="H46" t="n">
+        <v>1123254</v>
       </c>
     </row>
     <row r="47">
@@ -1372,16 +1652,22 @@
         <v>43422</v>
       </c>
       <c r="C47" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D47" t="n">
         <v>6.5</v>
       </c>
       <c r="E47" t="n">
-        <v>3.265714285714286</v>
+        <v>5.442857142857143</v>
       </c>
       <c r="F47" t="n">
-        <v>0.6685714285714287</v>
+        <v>1.114285714285714</v>
+      </c>
+      <c r="G47" t="n">
+        <v>10251.57142857143</v>
+      </c>
+      <c r="H47" t="n">
+        <v>1212043.285714286</v>
       </c>
     </row>
     <row r="48">
@@ -1398,10 +1684,16 @@
         <v>3.414285714285714</v>
       </c>
       <c r="E48" t="n">
-        <v>0.2314285714285714</v>
+        <v>0.3857142857142857</v>
       </c>
       <c r="F48" t="n">
-        <v>0.05142857142857143</v>
+        <v>0.08571428571428572</v>
+      </c>
+      <c r="G48" t="n">
+        <v>10154.85714285714</v>
+      </c>
+      <c r="H48" t="n">
+        <v>1126955.428571429</v>
       </c>
     </row>
     <row r="49">
@@ -1418,10 +1710,16 @@
         <v>7.685714285714285</v>
       </c>
       <c r="E49" t="n">
-        <v>0.1885714285714286</v>
+        <v>0.3142857142857143</v>
       </c>
       <c r="F49" t="n">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="G49" t="n">
+        <v>10104.14285714286</v>
+      </c>
+      <c r="H49" t="n">
+        <v>1241225.428571429</v>
       </c>
     </row>
     <row r="50">
@@ -1432,16 +1730,22 @@
         <v>43443</v>
       </c>
       <c r="C50" t="n">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D50" t="n">
         <v>8.571428571428571</v>
       </c>
       <c r="E50" t="n">
-        <v>0.7628571428571428</v>
+        <v>1.271428571428572</v>
       </c>
       <c r="F50" t="n">
-        <v>3.565714285714286</v>
+        <v>5.942857142857143</v>
+      </c>
+      <c r="G50" t="n">
+        <v>10082.42857142857</v>
+      </c>
+      <c r="H50" t="n">
+        <v>1084112.428571429</v>
       </c>
     </row>
     <row r="51">
@@ -1458,10 +1762,16 @@
         <v>1.942857142857143</v>
       </c>
       <c r="E51" t="n">
-        <v>1.542857142857143</v>
+        <v>2.571428571428572</v>
       </c>
       <c r="F51" t="n">
-        <v>0.5142857142857143</v>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="G51" t="n">
+        <v>10214.85714285714</v>
+      </c>
+      <c r="H51" t="n">
+        <v>948941.1428571428</v>
       </c>
     </row>
     <row r="52">
@@ -1478,10 +1788,16 @@
         <v>7.614285714285714</v>
       </c>
       <c r="E52" t="n">
-        <v>0.2485714285714286</v>
+        <v>0.4142857142857143</v>
       </c>
       <c r="F52" t="n">
-        <v>3.042857142857142</v>
+        <v>5.071428571428571</v>
+      </c>
+      <c r="G52" t="n">
+        <v>10121.14285714286</v>
+      </c>
+      <c r="H52" t="n">
+        <v>1126984</v>
       </c>
     </row>
     <row r="53">
@@ -1498,10 +1814,16 @@
         <v>4.971428571428571</v>
       </c>
       <c r="E53" t="n">
-        <v>0.7971428571428572</v>
+        <v>1.328571428571429</v>
       </c>
       <c r="F53" t="n">
-        <v>0.5057142857142857</v>
+        <v>0.8428571428571429</v>
+      </c>
+      <c r="G53" t="n">
+        <v>10305.85714285714</v>
+      </c>
+      <c r="H53" t="n">
+        <v>969826.8571428572</v>
       </c>
     </row>
     <row r="54">
@@ -1518,10 +1840,16 @@
         <v>6.314285714285715</v>
       </c>
       <c r="E54" t="n">
-        <v>0.5142857142857143</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="F54" t="n">
-        <v>0.3342857142857142</v>
+        <v>0.5571428571428572</v>
+      </c>
+      <c r="G54" t="n">
+        <v>10348.71428571429</v>
+      </c>
+      <c r="H54" t="n">
+        <v>1253984</v>
       </c>
     </row>
     <row r="55">
@@ -1538,10 +1866,16 @@
         <v>6.428571428571429</v>
       </c>
       <c r="E55" t="n">
-        <v>0.5742857142857142</v>
+        <v>0.9571428571428572</v>
       </c>
       <c r="F55" t="n">
-        <v>2.288571428571429</v>
+        <v>3.814285714285714</v>
+      </c>
+      <c r="G55" t="n">
+        <v>10202.71428571429</v>
+      </c>
+      <c r="H55" t="n">
+        <v>1095555.285714286</v>
       </c>
     </row>
     <row r="56">
@@ -1552,16 +1886,22 @@
         <v>43485</v>
       </c>
       <c r="C56" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D56" t="n">
         <v>2.3</v>
       </c>
       <c r="E56" t="n">
-        <v>2.194285714285714</v>
+        <v>3.657142857142857</v>
       </c>
       <c r="F56" t="n">
-        <v>1.002857142857143</v>
+        <v>1.671428571428571</v>
+      </c>
+      <c r="G56" t="n">
+        <v>10138.14285714286</v>
+      </c>
+      <c r="H56" t="n">
+        <v>983810.1428571428</v>
       </c>
     </row>
     <row r="57">
@@ -1578,10 +1918,16 @@
         <v>1.028571428571429</v>
       </c>
       <c r="E57" t="n">
-        <v>0.7285714285714285</v>
+        <v>1.214285714285714</v>
       </c>
       <c r="F57" t="n">
-        <v>2.151428571428571</v>
+        <v>3.585714285714286</v>
+      </c>
+      <c r="G57" t="n">
+        <v>10055.57142857143</v>
+      </c>
+      <c r="H57" t="n">
+        <v>698412.5714285715</v>
       </c>
     </row>
     <row r="58">
@@ -1598,10 +1944,16 @@
         <v>1.328571428571429</v>
       </c>
       <c r="E58" t="n">
-        <v>1.474285714285714</v>
+        <v>2.457142857142857</v>
       </c>
       <c r="F58" t="n">
-        <v>1.491428571428572</v>
+        <v>2.485714285714285</v>
+      </c>
+      <c r="G58" t="n">
+        <v>9999</v>
+      </c>
+      <c r="H58" t="n">
+        <v>983983.1428571428</v>
       </c>
     </row>
     <row r="59">
@@ -1618,10 +1970,16 @@
         <v>6.014285714285714</v>
       </c>
       <c r="E59" t="n">
-        <v>0.8485714285714285</v>
+        <v>1.414285714285714</v>
       </c>
       <c r="F59" t="n">
-        <v>4.654285714285714</v>
+        <v>7.757142857142858</v>
+      </c>
+      <c r="G59" t="n">
+        <v>10109.28571428571</v>
+      </c>
+      <c r="H59" t="n">
+        <v>1126696.857142857</v>
       </c>
     </row>
     <row r="60">
@@ -1638,10 +1996,16 @@
         <v>5.628571428571428</v>
       </c>
       <c r="E60" t="n">
-        <v>4.225714285714285</v>
+        <v>7.042857142857143</v>
       </c>
       <c r="F60" t="n">
-        <v>0.07714285714285715</v>
+        <v>0.1285714285714286</v>
+      </c>
+      <c r="G60" t="n">
+        <v>10282</v>
+      </c>
+      <c r="H60" t="n">
+        <v>840723.8571428572</v>
       </c>
     </row>
     <row r="61">
@@ -1652,16 +2016,22 @@
         <v>43520</v>
       </c>
       <c r="C61" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D61" t="n">
         <v>7.514285714285714</v>
       </c>
       <c r="E61" t="n">
-        <v>3.325714285714286</v>
+        <v>5.542857142857143</v>
       </c>
       <c r="F61" t="n">
-        <v>0.4285714285714285</v>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="G61" t="n">
+        <v>10278.42857142857</v>
+      </c>
+      <c r="H61" t="n">
+        <v>968404.7142857143</v>
       </c>
     </row>
     <row r="62">
@@ -1678,10 +2048,16 @@
         <v>8.285714285714286</v>
       </c>
       <c r="E62" t="n">
-        <v>2.94</v>
+        <v>4.899999999999999</v>
       </c>
       <c r="F62" t="n">
-        <v>1.02</v>
+        <v>1.7</v>
+      </c>
+      <c r="G62" t="n">
+        <v>10201.28571428571</v>
+      </c>
+      <c r="H62" t="n">
+        <v>400984</v>
       </c>
     </row>
     <row r="63">
@@ -1692,16 +2068,22 @@
         <v>43534</v>
       </c>
       <c r="C63" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D63" t="n">
         <v>8.27142857142857</v>
       </c>
       <c r="E63" t="n">
-        <v>2.357142857142857</v>
+        <v>3.928571428571428</v>
       </c>
       <c r="F63" t="n">
-        <v>2.94</v>
+        <v>4.899999999999999</v>
+      </c>
+      <c r="G63" t="n">
+        <v>10014</v>
+      </c>
+      <c r="H63" t="n">
+        <v>1255396.857142857</v>
       </c>
     </row>
     <row r="64">
@@ -1712,16 +2094,22 @@
         <v>43541</v>
       </c>
       <c r="C64" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D64" t="n">
         <v>7.757142857142857</v>
       </c>
       <c r="E64" t="n">
-        <v>1.268571428571429</v>
+        <v>2.114285714285714</v>
       </c>
       <c r="F64" t="n">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="G64" t="n">
+        <v>10057.85714285714</v>
+      </c>
+      <c r="H64" t="n">
+        <v>1125555.142857143</v>
       </c>
     </row>
     <row r="65">
@@ -1732,16 +2120,22 @@
         <v>43548</v>
       </c>
       <c r="C65" t="n">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="D65" t="n">
         <v>7.157142857142857</v>
       </c>
       <c r="E65" t="n">
-        <v>2.657142857142857</v>
+        <v>4.428571428571429</v>
       </c>
       <c r="F65" t="n">
-        <v>0.09428571428571429</v>
+        <v>0.1571428571428572</v>
+      </c>
+      <c r="G65" t="n">
+        <v>10286.85714285714</v>
+      </c>
+      <c r="H65" t="n">
+        <v>655540.5714285715</v>
       </c>
     </row>
     <row r="66">
@@ -1752,16 +2146,22 @@
         <v>43555</v>
       </c>
       <c r="C66" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D66" t="n">
         <v>8.742857142857144</v>
       </c>
       <c r="E66" t="n">
-        <v>3.24</v>
+        <v>5.399999999999999</v>
       </c>
       <c r="F66" t="n">
-        <v>0.08571428571428572</v>
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="G66" t="n">
+        <v>10289.14285714286</v>
+      </c>
+      <c r="H66" t="n">
+        <v>1125290.571428571</v>
       </c>
     </row>
     <row r="67">
@@ -1772,16 +2172,22 @@
         <v>43562</v>
       </c>
       <c r="C67" t="n">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D67" t="n">
         <v>8.800000000000001</v>
       </c>
       <c r="E67" t="n">
-        <v>3.78</v>
+        <v>6.3</v>
       </c>
       <c r="F67" t="n">
-        <v>0.4285714285714285</v>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="G67" t="n">
+        <v>10065.85714285714</v>
+      </c>
+      <c r="H67" t="n">
+        <v>98398.14285714286</v>
       </c>
     </row>
     <row r="68">
@@ -1792,16 +2198,22 @@
         <v>43569</v>
       </c>
       <c r="C68" t="n">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D68" t="n">
         <v>7.100000000000001</v>
       </c>
       <c r="E68" t="n">
-        <v>6.094285714285713</v>
+        <v>10.15714285714286</v>
       </c>
       <c r="F68" t="n">
         <v>0</v>
+      </c>
+      <c r="G68" t="n">
+        <v>10208.14285714286</v>
+      </c>
+      <c r="H68" t="n">
+        <v>671933.2857142857</v>
       </c>
     </row>
     <row r="69">
@@ -1812,16 +2224,22 @@
         <v>43576</v>
       </c>
       <c r="C69" t="n">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D69" t="n">
         <v>14.57142857142857</v>
       </c>
       <c r="E69" t="n">
-        <v>6.54</v>
+        <v>10.9</v>
       </c>
       <c r="F69" t="n">
         <v>0</v>
+      </c>
+      <c r="G69" t="n">
+        <v>10234.42857142857</v>
+      </c>
+      <c r="H69" t="n">
+        <v>526185.7142857143</v>
       </c>
     </row>
     <row r="70">
@@ -1832,16 +2250,22 @@
         <v>43583</v>
       </c>
       <c r="C70" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D70" t="n">
         <v>13.32857142857143</v>
       </c>
       <c r="E70" t="n">
-        <v>3.728571428571429</v>
+        <v>6.214285714285714</v>
       </c>
       <c r="F70" t="n">
-        <v>0.9171428571428571</v>
+        <v>1.528571428571428</v>
+      </c>
+      <c r="G70" t="n">
+        <v>10076.71428571429</v>
+      </c>
+      <c r="H70" t="n">
+        <v>666826.7142857143</v>
       </c>
     </row>
     <row r="71">
@@ -1858,10 +2282,16 @@
         <v>8.657142857142857</v>
       </c>
       <c r="E71" t="n">
-        <v>3.608571428571429</v>
+        <v>6.014285714285714</v>
       </c>
       <c r="F71" t="n">
-        <v>0.7885714285714286</v>
+        <v>1.314285714285714</v>
+      </c>
+      <c r="G71" t="n">
+        <v>10178.14285714286</v>
+      </c>
+      <c r="H71" t="n">
+        <v>982549.4285714285</v>
       </c>
     </row>
     <row r="72">
@@ -1878,10 +2308,16 @@
         <v>9.557142857142859</v>
       </c>
       <c r="E72" t="n">
-        <v>4.011428571428572</v>
+        <v>6.685714285714285</v>
       </c>
       <c r="F72" t="n">
-        <v>0.3428571428571429</v>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="G72" t="n">
+        <v>10137.71428571429</v>
+      </c>
+      <c r="H72" t="n">
+        <v>1126821.714285714</v>
       </c>
     </row>
     <row r="73">
@@ -1892,16 +2328,22 @@
         <v>43604</v>
       </c>
       <c r="C73" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D73" t="n">
         <v>12.38571428571429</v>
       </c>
       <c r="E73" t="n">
-        <v>5.554285714285714</v>
+        <v>9.257142857142856</v>
       </c>
       <c r="F73" t="n">
         <v>0</v>
+      </c>
+      <c r="G73" t="n">
+        <v>10197.57142857143</v>
+      </c>
+      <c r="H73" t="n">
+        <v>348124</v>
       </c>
     </row>
     <row r="74">
@@ -1912,16 +2354,22 @@
         <v>43611</v>
       </c>
       <c r="C74" t="n">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D74" t="n">
         <v>13.95714285714286</v>
       </c>
       <c r="E74" t="n">
-        <v>4.054285714285714</v>
+        <v>6.757142857142857</v>
       </c>
       <c r="F74" t="n">
-        <v>0.3</v>
+        <v>0.5</v>
+      </c>
+      <c r="G74" t="n">
+        <v>10150.85714285714</v>
+      </c>
+      <c r="H74" t="n">
+        <v>1268068.285714286</v>
       </c>
     </row>
     <row r="75">
@@ -1932,16 +2380,22 @@
         <v>43618</v>
       </c>
       <c r="C75" t="n">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D75" t="n">
         <v>16.27142857142857</v>
       </c>
       <c r="E75" t="n">
-        <v>5.322857142857143</v>
+        <v>8.871428571428572</v>
       </c>
       <c r="F75" t="n">
-        <v>0.5485714285714286</v>
+        <v>0.9142857142857144</v>
+      </c>
+      <c r="G75" t="n">
+        <v>10169.71428571429</v>
+      </c>
+      <c r="H75" t="n">
+        <v>1076983.857142857</v>
       </c>
     </row>
     <row r="76">
@@ -1952,16 +2406,22 @@
         <v>43625</v>
       </c>
       <c r="C76" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D76" t="n">
         <v>16.02857142857143</v>
       </c>
       <c r="E76" t="n">
-        <v>3.214285714285714</v>
+        <v>5.357142857142857</v>
       </c>
       <c r="F76" t="n">
-        <v>0.7285714285714285</v>
+        <v>1.214285714285714</v>
+      </c>
+      <c r="G76" t="n">
+        <v>10119.71428571429</v>
+      </c>
+      <c r="H76" t="n">
+        <v>1253822.428571429</v>
       </c>
     </row>
     <row r="77">
@@ -1972,16 +2432,22 @@
         <v>43632</v>
       </c>
       <c r="C77" t="n">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D77" t="n">
         <v>15.91428571428571</v>
       </c>
       <c r="E77" t="n">
-        <v>3.771428571428571</v>
+        <v>6.285714285714286</v>
       </c>
       <c r="F77" t="n">
-        <v>1.08</v>
+        <v>1.8</v>
+      </c>
+      <c r="G77" t="n">
+        <v>10128.71428571429</v>
+      </c>
+      <c r="H77" t="n">
+        <v>1123953.428571429</v>
       </c>
     </row>
     <row r="78">
@@ -1992,16 +2458,22 @@
         <v>43639</v>
       </c>
       <c r="C78" t="n">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D78" t="n">
         <v>18.61428571428572</v>
       </c>
       <c r="E78" t="n">
-        <v>6.008571428571429</v>
+        <v>10.01428571428571</v>
       </c>
       <c r="F78" t="n">
-        <v>0.2485714285714286</v>
+        <v>0.4142857142857143</v>
+      </c>
+      <c r="G78" t="n">
+        <v>10159.85714285714</v>
+      </c>
+      <c r="H78" t="n">
+        <v>539332.2857142857</v>
       </c>
     </row>
     <row r="79">
@@ -2012,16 +2484,22 @@
         <v>43646</v>
       </c>
       <c r="C79" t="n">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D79" t="n">
         <v>21.21428571428572</v>
       </c>
       <c r="E79" t="n">
-        <v>6.942857142857143</v>
+        <v>11.57142857142857</v>
       </c>
       <c r="F79" t="n">
         <v>0</v>
+      </c>
+      <c r="G79" t="n">
+        <v>10209</v>
+      </c>
+      <c r="H79" t="n">
+        <v>1236186.142857143</v>
       </c>
     </row>
     <row r="80">
@@ -2032,16 +2510,22 @@
         <v>43653</v>
       </c>
       <c r="C80" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D80" t="n">
         <v>16.55714285714286</v>
       </c>
       <c r="E80" t="n">
-        <v>5.777142857142857</v>
+        <v>9.62857142857143</v>
       </c>
       <c r="F80" t="n">
-        <v>0.2142857142857143</v>
+        <v>0.3571428571428572</v>
+      </c>
+      <c r="G80" t="n">
+        <v>10196</v>
+      </c>
+      <c r="H80" t="n">
+        <v>619495.1428571428</v>
       </c>
     </row>
     <row r="81">
@@ -2058,10 +2542,16 @@
         <v>15.9</v>
       </c>
       <c r="E81" t="n">
-        <v>2.631428571428571</v>
+        <v>4.385714285714285</v>
       </c>
       <c r="F81" t="n">
-        <v>0.8657142857142858</v>
+        <v>1.442857142857143</v>
+      </c>
+      <c r="G81" t="n">
+        <v>10178.57142857143</v>
+      </c>
+      <c r="H81" t="n">
+        <v>1083984</v>
       </c>
     </row>
     <row r="82">
@@ -2072,16 +2562,22 @@
         <v>43667</v>
       </c>
       <c r="C82" t="n">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D82" t="n">
         <v>17.85714285714286</v>
       </c>
       <c r="E82" t="n">
-        <v>3.214285714285714</v>
+        <v>5.357142857142857</v>
       </c>
       <c r="F82" t="n">
-        <v>0.3342857142857142</v>
+        <v>0.5571428571428572</v>
+      </c>
+      <c r="G82" t="n">
+        <v>10156.28571428571</v>
+      </c>
+      <c r="H82" t="n">
+        <v>1251266.714285714</v>
       </c>
     </row>
     <row r="83">
@@ -2098,10 +2594,16 @@
         <v>24.42857142857143</v>
       </c>
       <c r="E83" t="n">
-        <v>6.411428571428572</v>
+        <v>10.68571428571429</v>
       </c>
       <c r="F83" t="n">
-        <v>0.04285714285714286</v>
+        <v>0.07142857142857142</v>
+      </c>
+      <c r="G83" t="n">
+        <v>10120.42857142857</v>
+      </c>
+      <c r="H83" t="n">
+        <v>876225.4285714285</v>
       </c>
     </row>
     <row r="84">
@@ -2118,10 +2620,16 @@
         <v>18.94285714285714</v>
       </c>
       <c r="E84" t="n">
-        <v>4.217142857142857</v>
+        <v>7.028571428571429</v>
       </c>
       <c r="F84" t="n">
-        <v>0.2828571428571429</v>
+        <v>0.4714285714285714</v>
+      </c>
+      <c r="G84" t="n">
+        <v>10143.42857142857</v>
+      </c>
+      <c r="H84" t="n">
+        <v>336668</v>
       </c>
     </row>
     <row r="85">
@@ -2132,16 +2640,22 @@
         <v>43688</v>
       </c>
       <c r="C85" t="n">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D85" t="n">
         <v>19.38571428571428</v>
       </c>
       <c r="E85" t="n">
-        <v>4.225714285714285</v>
+        <v>7.042857142857143</v>
       </c>
       <c r="F85" t="n">
-        <v>0.3857142857142857</v>
+        <v>0.6428571428571429</v>
+      </c>
+      <c r="G85" t="n">
+        <v>10093</v>
+      </c>
+      <c r="H85" t="n">
+        <v>1106547.857142857</v>
       </c>
     </row>
     <row r="86">
@@ -2158,10 +2672,16 @@
         <v>16.54285714285714</v>
       </c>
       <c r="E86" t="n">
-        <v>2.871428571428571</v>
+        <v>4.785714285714286</v>
       </c>
       <c r="F86" t="n">
-        <v>1.988571428571429</v>
+        <v>3.314285714285714</v>
+      </c>
+      <c r="G86" t="n">
+        <v>10118.42857142857</v>
+      </c>
+      <c r="H86" t="n">
+        <v>811126.5714285715</v>
       </c>
     </row>
     <row r="87">
@@ -2178,10 +2698,16 @@
         <v>17.45714285714286</v>
       </c>
       <c r="E87" t="n">
-        <v>6.857142857142857</v>
+        <v>11.42857142857143</v>
       </c>
       <c r="F87" t="n">
-        <v>0.008571428571428572</v>
+        <v>0.01428571428571429</v>
+      </c>
+      <c r="G87" t="n">
+        <v>10221.28571428571</v>
+      </c>
+      <c r="H87" t="n">
+        <v>462231.8571428572</v>
       </c>
     </row>
     <row r="88">
@@ -2192,16 +2718,22 @@
         <v>43709</v>
       </c>
       <c r="C88" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D88" t="n">
         <v>20.1</v>
       </c>
       <c r="E88" t="n">
-        <v>5.048571428571429</v>
+        <v>8.414285714285715</v>
       </c>
       <c r="F88" t="n">
         <v>0</v>
+      </c>
+      <c r="G88" t="n">
+        <v>10164.42857142857</v>
+      </c>
+      <c r="H88" t="n">
+        <v>182408</v>
       </c>
     </row>
     <row r="89">
@@ -2218,10 +2750,16 @@
         <v>14.45714285714286</v>
       </c>
       <c r="E89" t="n">
-        <v>3.334285714285714</v>
+        <v>5.557142857142857</v>
       </c>
       <c r="F89" t="n">
-        <v>0.6857142857142857</v>
+        <v>1.142857142857143</v>
+      </c>
+      <c r="G89" t="n">
+        <v>10198.85714285714</v>
+      </c>
+      <c r="H89" t="n">
+        <v>680696.1428571428</v>
       </c>
     </row>
     <row r="90">
@@ -2238,10 +2776,16 @@
         <v>14.57142857142857</v>
       </c>
       <c r="E90" t="n">
-        <v>3.968571428571429</v>
+        <v>6.614285714285714</v>
       </c>
       <c r="F90" t="n">
-        <v>0.6514285714285714</v>
+        <v>1.085714285714286</v>
+      </c>
+      <c r="G90" t="n">
+        <v>10239.71428571429</v>
+      </c>
+      <c r="H90" t="n">
+        <v>655221</v>
       </c>
     </row>
     <row r="91">
@@ -2258,10 +2802,16 @@
         <v>13.4</v>
       </c>
       <c r="E91" t="n">
-        <v>4.037142857142856</v>
+        <v>6.728571428571428</v>
       </c>
       <c r="F91" t="n">
-        <v>0.7028571428571428</v>
+        <v>1.171428571428571</v>
+      </c>
+      <c r="G91" t="n">
+        <v>10222.14285714286</v>
+      </c>
+      <c r="H91" t="n">
+        <v>1252486.571428571</v>
       </c>
     </row>
     <row r="92">
@@ -2278,10 +2828,16 @@
         <v>15.45714285714286</v>
       </c>
       <c r="E92" t="n">
-        <v>1.208571428571428</v>
+        <v>2.014285714285714</v>
       </c>
       <c r="F92" t="n">
-        <v>2.58</v>
+        <v>4.3</v>
+      </c>
+      <c r="G92" t="n">
+        <v>10063.28571428571</v>
+      </c>
+      <c r="H92" t="n">
+        <v>1126969.714285714</v>
       </c>
     </row>
     <row r="93">
@@ -2298,10 +2854,16 @@
         <v>11.54285714285714</v>
       </c>
       <c r="E93" t="n">
-        <v>2.228571428571429</v>
+        <v>3.714285714285714</v>
       </c>
       <c r="F93" t="n">
-        <v>2.537142857142857</v>
+        <v>4.228571428571429</v>
+      </c>
+      <c r="G93" t="n">
+        <v>10099.71428571429</v>
+      </c>
+      <c r="H93" t="n">
+        <v>1122555.428571429</v>
       </c>
     </row>
     <row r="94">
@@ -2318,10 +2880,16 @@
         <v>12.95714285714286</v>
       </c>
       <c r="E94" t="n">
-        <v>0.7542857142857142</v>
+        <v>1.257142857142857</v>
       </c>
       <c r="F94" t="n">
-        <v>2.588571428571429</v>
+        <v>4.314285714285714</v>
+      </c>
+      <c r="G94" t="n">
+        <v>10089.28571428571</v>
+      </c>
+      <c r="H94" t="n">
+        <v>1240984</v>
       </c>
     </row>
     <row r="95">
@@ -2332,16 +2900,22 @@
         <v>43758</v>
       </c>
       <c r="C95" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D95" t="n">
         <v>13.08571428571429</v>
       </c>
       <c r="E95" t="n">
-        <v>1.508571428571429</v>
+        <v>2.514285714285715</v>
       </c>
       <c r="F95" t="n">
-        <v>1.431428571428571</v>
+        <v>2.385714285714286</v>
+      </c>
+      <c r="G95" t="n">
+        <v>10068</v>
+      </c>
+      <c r="H95" t="n">
+        <v>1268255.428571429</v>
       </c>
     </row>
     <row r="96">
@@ -2358,10 +2932,16 @@
         <v>12.75714285714286</v>
       </c>
       <c r="E96" t="n">
-        <v>1.937142857142857</v>
+        <v>3.228571428571429</v>
       </c>
       <c r="F96" t="n">
-        <v>0.5914285714285715</v>
+        <v>0.9857142857142858</v>
+      </c>
+      <c r="G96" t="n">
+        <v>10152.42857142857</v>
+      </c>
+      <c r="H96" t="n">
+        <v>1254125.285714286</v>
       </c>
     </row>
     <row r="97">
@@ -2378,10 +2958,16 @@
         <v>7.357142857142857</v>
       </c>
       <c r="E97" t="n">
-        <v>3.06</v>
+        <v>5.100000000000001</v>
       </c>
       <c r="F97" t="n">
-        <v>1.697142857142857</v>
+        <v>2.828571428571429</v>
+      </c>
+      <c r="G97" t="n">
+        <v>10106.14285714286</v>
+      </c>
+      <c r="H97" t="n">
+        <v>743412.4285714285</v>
       </c>
     </row>
     <row r="98">
@@ -2398,10 +2984,16 @@
         <v>7.114285714285714</v>
       </c>
       <c r="E98" t="n">
-        <v>2.082857142857143</v>
+        <v>3.471428571428572</v>
       </c>
       <c r="F98" t="n">
-        <v>0.9342857142857143</v>
+        <v>1.557142857142857</v>
+      </c>
+      <c r="G98" t="n">
+        <v>10010</v>
+      </c>
+      <c r="H98" t="n">
+        <v>1269453</v>
       </c>
     </row>
     <row r="99">
@@ -2418,10 +3010,16 @@
         <v>5</v>
       </c>
       <c r="E99" t="n">
-        <v>0.8828571428571428</v>
+        <v>1.471428571428572</v>
       </c>
       <c r="F99" t="n">
-        <v>1.234285714285714</v>
+        <v>2.057142857142857</v>
+      </c>
+      <c r="G99" t="n">
+        <v>10033.57142857143</v>
+      </c>
+      <c r="H99" t="n">
+        <v>1254126.714285714</v>
       </c>
     </row>
     <row r="100">
@@ -2438,10 +3036,16 @@
         <v>4.742857142857143</v>
       </c>
       <c r="E100" t="n">
-        <v>1.911428571428571</v>
+        <v>3.185714285714286</v>
       </c>
       <c r="F100" t="n">
-        <v>0.8142857142857143</v>
+        <v>1.357142857142857</v>
+      </c>
+      <c r="G100" t="n">
+        <v>10085.42857142857</v>
+      </c>
+      <c r="H100" t="n">
+        <v>1221255.428571429</v>
       </c>
     </row>
     <row r="101">
@@ -2458,10 +3062,16 @@
         <v>5.985714285714286</v>
       </c>
       <c r="E101" t="n">
-        <v>1.602857142857143</v>
+        <v>2.671428571428572</v>
       </c>
       <c r="F101" t="n">
-        <v>1.817142857142857</v>
+        <v>3.028571428571428</v>
+      </c>
+      <c r="G101" t="n">
+        <v>10064.85714285714</v>
+      </c>
+      <c r="H101" t="n">
+        <v>1126918.142857143</v>
       </c>
     </row>
     <row r="102">
@@ -2478,10 +3088,16 @@
         <v>5.371428571428572</v>
       </c>
       <c r="E102" t="n">
-        <v>1.534285714285714</v>
+        <v>2.557142857142857</v>
       </c>
       <c r="F102" t="n">
-        <v>1.774285714285714</v>
+        <v>2.957142857142857</v>
+      </c>
+      <c r="G102" t="n">
+        <v>10159.14285714286</v>
+      </c>
+      <c r="H102" t="n">
+        <v>918412.4285714285</v>
       </c>
     </row>
     <row r="103">
@@ -2498,10 +3114,16 @@
         <v>5.814285714285715</v>
       </c>
       <c r="E103" t="n">
-        <v>1.568571428571429</v>
+        <v>2.614285714285714</v>
       </c>
       <c r="F103" t="n">
-        <v>2.151428571428571</v>
+        <v>3.585714285714286</v>
+      </c>
+      <c r="G103" t="n">
+        <v>9982.142857142857</v>
+      </c>
+      <c r="H103" t="n">
+        <v>969553.7142857143</v>
       </c>
     </row>
     <row r="104">
@@ -2518,10 +3140,16 @@
         <v>8.514285714285714</v>
       </c>
       <c r="E104" t="n">
-        <v>1.002857142857143</v>
+        <v>1.671428571428571</v>
       </c>
       <c r="F104" t="n">
-        <v>1.791428571428571</v>
+        <v>2.985714285714285</v>
+      </c>
+      <c r="G104" t="n">
+        <v>9970.857142857143</v>
+      </c>
+      <c r="H104" t="n">
+        <v>1268396.857142857</v>
       </c>
     </row>
     <row r="105">
@@ -2538,10 +3166,16 @@
         <v>4.885714285714286</v>
       </c>
       <c r="E105" t="n">
-        <v>1.397142857142857</v>
+        <v>2.328571428571429</v>
       </c>
       <c r="F105" t="n">
-        <v>1.011428571428571</v>
+        <v>1.685714285714286</v>
+      </c>
+      <c r="G105" t="n">
+        <v>10230.42857142857</v>
+      </c>
+      <c r="H105" t="n">
+        <v>1125512.571428571</v>
       </c>
     </row>
     <row r="106">
@@ -2558,10 +3192,16 @@
         <v>4.957142857142857</v>
       </c>
       <c r="E106" t="n">
-        <v>1.02</v>
+        <v>1.7</v>
       </c>
       <c r="F106" t="n">
-        <v>0.7028571428571428</v>
+        <v>1.171428571428571</v>
+      </c>
+      <c r="G106" t="n">
+        <v>10285.71428571429</v>
+      </c>
+      <c r="H106" t="n">
+        <v>541255.4285714285</v>
       </c>
     </row>
     <row r="107">
@@ -2578,10 +3218,16 @@
         <v>7.828571428571428</v>
       </c>
       <c r="E107" t="n">
-        <v>0.5914285714285715</v>
+        <v>0.9857142857142858</v>
       </c>
       <c r="F107" t="n">
-        <v>1.697142857142857</v>
+        <v>2.828571428571429</v>
+      </c>
+      <c r="G107" t="n">
+        <v>10208.85714285714</v>
+      </c>
+      <c r="H107" t="n">
+        <v>1098384</v>
       </c>
     </row>
     <row r="108">
@@ -2598,10 +3244,16 @@
         <v>7.328571428571428</v>
       </c>
       <c r="E108" t="n">
-        <v>1.74</v>
+        <v>2.899999999999999</v>
       </c>
       <c r="F108" t="n">
-        <v>1.457142857142857</v>
+        <v>2.428571428571428</v>
+      </c>
+      <c r="G108" t="n">
+        <v>10181.71428571429</v>
+      </c>
+      <c r="H108" t="n">
+        <v>1123820.285714286</v>
       </c>
     </row>
     <row r="109">
@@ -2618,10 +3270,16 @@
         <v>3.071428571428572</v>
       </c>
       <c r="E109" t="n">
-        <v>0.5657142857142857</v>
+        <v>0.9428571428571428</v>
       </c>
       <c r="F109" t="n">
-        <v>0.5228571428571429</v>
+        <v>0.8714285714285713</v>
+      </c>
+      <c r="G109" t="n">
+        <v>10306.57142857143</v>
+      </c>
+      <c r="H109" t="n">
+        <v>1098126.857142857</v>
       </c>
     </row>
     <row r="110">
@@ -2638,10 +3296,16 @@
         <v>8.357142857142858</v>
       </c>
       <c r="E110" t="n">
-        <v>0.7028571428571428</v>
+        <v>1.171428571428571</v>
       </c>
       <c r="F110" t="n">
-        <v>1.894285714285715</v>
+        <v>3.157142857142857</v>
+      </c>
+      <c r="G110" t="n">
+        <v>10034.42857142857</v>
+      </c>
+      <c r="H110" t="n">
+        <v>1255554</v>
       </c>
     </row>
     <row r="111">
@@ -2658,10 +3322,16 @@
         <v>6.428571428571429</v>
       </c>
       <c r="E111" t="n">
-        <v>1.962857142857143</v>
+        <v>3.271428571428572</v>
       </c>
       <c r="F111" t="n">
-        <v>1.088571428571429</v>
+        <v>1.814285714285714</v>
+      </c>
+      <c r="G111" t="n">
+        <v>10190.28571428571</v>
+      </c>
+      <c r="H111" t="n">
+        <v>1082312.571428571</v>
       </c>
     </row>
     <row r="112">
@@ -2678,10 +3348,16 @@
         <v>7.928571428571429</v>
       </c>
       <c r="E112" t="n">
-        <v>0.9171428571428571</v>
+        <v>1.528571428571428</v>
       </c>
       <c r="F112" t="n">
-        <v>1.594285714285714</v>
+        <v>2.657142857142857</v>
+      </c>
+      <c r="G112" t="n">
+        <v>10056.85714285714</v>
+      </c>
+      <c r="H112" t="n">
+        <v>1254126.857142857</v>
       </c>
     </row>
     <row r="113">
@@ -2698,10 +3374,16 @@
         <v>7.899999999999999</v>
       </c>
       <c r="E113" t="n">
-        <v>1.68</v>
+        <v>2.8</v>
       </c>
       <c r="F113" t="n">
-        <v>1.997142857142857</v>
+        <v>3.328571428571429</v>
+      </c>
+      <c r="G113" t="n">
+        <v>10157.57142857143</v>
+      </c>
+      <c r="H113" t="n">
+        <v>825526.7142857143</v>
       </c>
     </row>
     <row r="114">
@@ -2718,10 +3400,16 @@
         <v>5.742857142857142</v>
       </c>
       <c r="E114" t="n">
-        <v>1.465714285714286</v>
+        <v>2.442857142857143</v>
       </c>
       <c r="F114" t="n">
-        <v>2.828571428571429</v>
+        <v>4.714285714285714</v>
+      </c>
+      <c r="G114" t="n">
+        <v>10000.14285714286</v>
+      </c>
+      <c r="H114" t="n">
+        <v>1239681</v>
       </c>
     </row>
     <row r="115">
@@ -2738,10 +3426,16 @@
         <v>6.2</v>
       </c>
       <c r="E115" t="n">
-        <v>1.834285714285714</v>
+        <v>3.057142857142857</v>
       </c>
       <c r="F115" t="n">
-        <v>2.391428571428571</v>
+        <v>3.985714285714285</v>
+      </c>
+      <c r="G115" t="n">
+        <v>10029.28571428571</v>
+      </c>
+      <c r="H115" t="n">
+        <v>1054121.142857143</v>
       </c>
     </row>
     <row r="116">
@@ -2758,10 +3452,16 @@
         <v>8.6</v>
       </c>
       <c r="E116" t="n">
-        <v>2.1</v>
+        <v>3.5</v>
       </c>
       <c r="F116" t="n">
-        <v>2.597142857142857</v>
+        <v>4.328571428571428</v>
+      </c>
+      <c r="G116" t="n">
+        <v>10111.71428571429</v>
+      </c>
+      <c r="H116" t="n">
+        <v>1269254</v>
       </c>
     </row>
     <row r="117">
@@ -2778,10 +3478,16 @@
         <v>7.285714285714286</v>
       </c>
       <c r="E117" t="n">
-        <v>3.445714285714286</v>
+        <v>5.742857142857143</v>
       </c>
       <c r="F117" t="n">
         <v>0</v>
+      </c>
+      <c r="G117" t="n">
+        <v>10267.57142857143</v>
+      </c>
+      <c r="H117" t="n">
+        <v>696942.8571428572</v>
       </c>
     </row>
     <row r="118">
@@ -2798,10 +3504,16 @@
         <v>6.042857142857143</v>
       </c>
       <c r="E118" t="n">
-        <v>6.745714285714286</v>
+        <v>11.24285714285714</v>
       </c>
       <c r="F118" t="n">
         <v>0</v>
+      </c>
+      <c r="G118" t="n">
+        <v>10273.85714285714</v>
+      </c>
+      <c r="H118" t="n">
+        <v>190146</v>
       </c>
     </row>
     <row r="119">
@@ -2818,10 +3530,16 @@
         <v>6.471428571428571</v>
       </c>
       <c r="E119" t="n">
-        <v>4.577142857142857</v>
+        <v>7.628571428571428</v>
       </c>
       <c r="F119" t="n">
-        <v>0.04285714285714286</v>
+        <v>0.07142857142857142</v>
+      </c>
+      <c r="G119" t="n">
+        <v>10222.28571428571</v>
+      </c>
+      <c r="H119" t="n">
+        <v>722645.7142857143</v>
       </c>
     </row>
     <row r="120">
@@ -2838,10 +3556,16 @@
         <v>13.21428571428571</v>
       </c>
       <c r="E120" t="n">
-        <v>6.548571428571429</v>
+        <v>10.91428571428571</v>
       </c>
       <c r="F120" t="n">
-        <v>0.06857142857142857</v>
+        <v>0.1142857142857143</v>
+      </c>
+      <c r="G120" t="n">
+        <v>10236.14285714286</v>
+      </c>
+      <c r="H120" t="n">
+        <v>507682</v>
       </c>
     </row>
     <row r="121">
@@ -2852,16 +3576,22 @@
         <v>43940</v>
       </c>
       <c r="C121" t="n">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D121" t="n">
         <v>9.971428571428572</v>
       </c>
       <c r="E121" t="n">
-        <v>5.314285714285715</v>
+        <v>8.857142857142858</v>
       </c>
       <c r="F121" t="n">
-        <v>0.1542857142857143</v>
+        <v>0.2571428571428572</v>
+      </c>
+      <c r="G121" t="n">
+        <v>10206.71428571429</v>
+      </c>
+      <c r="H121" t="n">
+        <v>1106610.142857143</v>
       </c>
     </row>
     <row r="122">
@@ -2878,10 +3608,16 @@
         <v>12.68571428571429</v>
       </c>
       <c r="E122" t="n">
-        <v>7.208571428571429</v>
+        <v>12.01428571428571</v>
       </c>
       <c r="F122" t="n">
         <v>0</v>
+      </c>
+      <c r="G122" t="n">
+        <v>10169.85714285714</v>
+      </c>
+      <c r="H122" t="n">
+        <v>678.5714285714286</v>
       </c>
     </row>
     <row r="123">
@@ -2898,10 +3634,16 @@
         <v>10.97142857142857</v>
       </c>
       <c r="E123" t="n">
-        <v>3.068571428571429</v>
+        <v>5.114285714285714</v>
       </c>
       <c r="F123" t="n">
-        <v>1.688571428571429</v>
+        <v>2.814285714285715</v>
+      </c>
+      <c r="G123" t="n">
+        <v>10055.28571428571</v>
+      </c>
+      <c r="H123" t="n">
+        <v>698252.4285714285</v>
       </c>
     </row>
     <row r="124">
@@ -2912,16 +3654,22 @@
         <v>43961</v>
       </c>
       <c r="C124" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D124" t="n">
         <v>12.44285714285714</v>
       </c>
       <c r="E124" t="n">
-        <v>7.071428571428571</v>
+        <v>11.78571428571429</v>
       </c>
       <c r="F124" t="n">
-        <v>0.09428571428571429</v>
+        <v>0.1571428571428572</v>
+      </c>
+      <c r="G124" t="n">
+        <v>10186.71428571429</v>
+      </c>
+      <c r="H124" t="n">
+        <v>444949.5714285714</v>
       </c>
     </row>
     <row r="125">
@@ -2938,10 +3686,16 @@
         <v>8.685714285714285</v>
       </c>
       <c r="E125" t="n">
-        <v>5.537142857142856</v>
+        <v>9.228571428571428</v>
       </c>
       <c r="F125" t="n">
-        <v>0.06</v>
+        <v>0.09999999999999999</v>
+      </c>
+      <c r="G125" t="n">
+        <v>10199.42857142857</v>
+      </c>
+      <c r="H125" t="n">
+        <v>777495</v>
       </c>
     </row>
     <row r="126">
@@ -2952,16 +3706,22 @@
         <v>43975</v>
       </c>
       <c r="C126" t="n">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D126" t="n">
         <v>16.38571428571429</v>
       </c>
       <c r="E126" t="n">
-        <v>5.571428571428571</v>
+        <v>9.285714285714286</v>
       </c>
       <c r="F126" t="n">
-        <v>0.4371428571428572</v>
+        <v>0.7285714285714285</v>
+      </c>
+      <c r="G126" t="n">
+        <v>10222</v>
+      </c>
+      <c r="H126" t="n">
+        <v>1065123.857142857</v>
       </c>
     </row>
     <row r="127">
@@ -2978,10 +3738,16 @@
         <v>16</v>
       </c>
       <c r="E127" t="n">
-        <v>8.442857142857143</v>
+        <v>14.07142857142857</v>
       </c>
       <c r="F127" t="n">
         <v>0</v>
+      </c>
+      <c r="G127" t="n">
+        <v>10303.42857142857</v>
+      </c>
+      <c r="H127" t="n">
+        <v>518873.5714285714</v>
       </c>
     </row>
   </sheetData>

</xml_diff>